<commit_message>
UD4 add points function
</commit_message>
<xml_diff>
--- a/Universal_Driver_soft/UD_v4/Map Registers UD4.xlsx
+++ b/Universal_Driver_soft/UD_v4/Map Registers UD4.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF64074-DA9A-47C4-93BC-61E716CC6C8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB134FC4-AFF8-4A15-8FBE-EF2202D4C34B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-13068" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="143">
   <si>
     <t>Десятичная</t>
   </si>
@@ -519,6 +519,165 @@
 D0 - тип мотора
 N0 -</t>
     </r>
+  </si>
+  <si>
+    <t>0x12</t>
+  </si>
+  <si>
+    <t>0x13</t>
+  </si>
+  <si>
+    <t>0x14</t>
+  </si>
+  <si>
+    <t>0x15</t>
+  </si>
+  <si>
+    <t>0x16</t>
+  </si>
+  <si>
+    <t>0x17</t>
+  </si>
+  <si>
+    <t>0x18</t>
+  </si>
+  <si>
+    <t>0x19</t>
+  </si>
+  <si>
+    <t>savePoint</t>
+  </si>
+  <si>
+    <t>getPosition</t>
+  </si>
+  <si>
+    <t>Сохранить текущую позицию как точку</t>
+  </si>
+  <si>
+    <t>0-9</t>
+  </si>
+  <si>
+    <t>C20A0D3N0x</t>
+  </si>
+  <si>
+    <t>resetPosition</t>
+  </si>
+  <si>
+    <t>Сброс текущей позиции</t>
+  </si>
+  <si>
+    <t>C22A0D0N0x</t>
+  </si>
+  <si>
+    <t>setPosition</t>
+  </si>
+  <si>
+    <t>Установить текущую позицию</t>
+  </si>
+  <si>
+    <t>0-32766</t>
+  </si>
+  <si>
+    <t>C23A0D1000N0x</t>
+  </si>
+  <si>
+    <t>gotoPoint</t>
+  </si>
+  <si>
+    <t>Перейти на точку</t>
+  </si>
+  <si>
+    <t>C24A0D5N0x</t>
+  </si>
+  <si>
+    <t>getPoints</t>
+  </si>
+  <si>
+    <t>Получить массив точек</t>
+  </si>
+  <si>
+    <t>Возвращает массив сохраненных точек</t>
+  </si>
+  <si>
+    <t>C25A1D0N0x</t>
+  </si>
+  <si>
+    <t>C22A0D0N0x C22 - команда A0 - выполнить D0 - N0 -</t>
+  </si>
+  <si>
+    <t>C23A0D1000N0x C23 - команда A0 - записать D1000 - позиция N0 -</t>
+  </si>
+  <si>
+    <t>C24A0D5N0x C24 - команда A0 - выполнить D5 - номер точки N0 -</t>
+  </si>
+  <si>
+    <t>C25A1D0N0x C25 - команда A1 - прочитать D0 - N0 -</t>
+  </si>
+  <si>
+    <t>C20A0D3N0x C20 - команда A0 - записать D3 - номер точки N0 -</t>
+  </si>
+  <si>
+    <t>Получить текущую позицию в шагах и текущую точку</t>
+  </si>
+  <si>
+    <t>C21A1D0N0x - получить позицию C21A2D0N0x - получить текущую точку C21A3D0N0x - получить статус калибровки</t>
+  </si>
+  <si>
+    <t>При A1: текущая позиция в шагах При A2: номер текущей точки (0-9) При A3: статус калибровки (0/1)</t>
+  </si>
+  <si>
+    <t>C21A1D0N0x C21A2D0N0x C21A3D0N0x</t>
+  </si>
+  <si>
+    <t>0x1B</t>
+  </si>
+  <si>
+    <t>gotoPosition</t>
+  </si>
+  <si>
+    <t>Перейти на позицию в шагах</t>
+  </si>
+  <si>
+    <t>C27A0D1000N0x C27 - команда A0 - выполнить D1000 - позиция N0 -</t>
+  </si>
+  <si>
+    <t>C27A0D1000N0x</t>
+  </si>
+  <si>
+    <t>0x1C</t>
+  </si>
+  <si>
+    <t>getMaxPosition</t>
+  </si>
+  <si>
+    <t>Получить максимальную позицию</t>
+  </si>
+  <si>
+    <t>C28A1D0N0x C28 - команда A1 - прочитать D0 - N0 -</t>
+  </si>
+  <si>
+    <t>Возвращает максимальную доступную позицию</t>
+  </si>
+  <si>
+    <t>C28A1D0N0x</t>
+  </si>
+  <si>
+    <t>0x1D</t>
+  </si>
+  <si>
+    <t>getMinPosition</t>
+  </si>
+  <si>
+    <t>Получить минимальную позицию</t>
+  </si>
+  <si>
+    <t>C29A1D0N0x C29 - команда A1 - прочитать D0 - N0 -</t>
+  </si>
+  <si>
+    <t>Возвращает минимальную доступную позицию</t>
+  </si>
+  <si>
+    <t>C29A1D0N0x</t>
   </si>
 </sst>
 </file>
@@ -674,13 +833,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -708,8 +864,17 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1057,8 +1222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1082,221 +1247,221 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:10" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="4" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="189.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>1</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6" t="s">
+      <c r="E4" s="5"/>
+      <c r="F4" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="11" t="s">
+      <c r="H4" s="5"/>
+      <c r="I4" s="10" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="156" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>2</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6" t="s">
+      <c r="E5" s="5"/>
+      <c r="F5" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:10" ht="114" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>3</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6" t="s">
+      <c r="G6" s="5"/>
+      <c r="H6" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="5" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="129" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>4</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6" t="s">
+      <c r="G7" s="5"/>
+      <c r="H7" s="5" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="229.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>5</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6" t="s">
+      <c r="E8" s="5"/>
+      <c r="F8" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="6"/>
+      <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="108" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>6</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6" t="s">
+      <c r="E9" s="5"/>
+      <c r="F9" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6" t="s">
+      <c r="G9" s="5"/>
+      <c r="H9" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="I9" s="6"/>
+      <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>7</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6" t="s">
+      <c r="E10" s="5"/>
+      <c r="F10" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6" t="s">
+      <c r="G10" s="5"/>
+      <c r="H10" s="5" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="134.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>8</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6" t="s">
+      <c r="E11" s="5"/>
+      <c r="F11" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G11" s="6"/>
+      <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:10" ht="222" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
@@ -1311,14 +1476,14 @@
       <c r="D12" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6" t="s">
+      <c r="E12" s="5"/>
+      <c r="F12" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="9" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1327,265 +1492,406 @@
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6" t="s">
+      <c r="E13" s="5"/>
+      <c r="F13" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="H13" s="6"/>
+      <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:10" ht="116.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <v>10</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="6" t="s">
+      <c r="E14" s="7"/>
+      <c r="F14" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="G14" s="8"/>
+      <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:10" ht="141" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="5">
         <v>11</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6" t="s">
+      <c r="E15" s="5"/>
+      <c r="F15" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="G15" s="6"/>
+      <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="87" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
         <v>12</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6" t="s">
+      <c r="E16" s="5"/>
+      <c r="F16" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="G16" s="6"/>
-    </row>
-    <row r="17" spans="1:7" ht="166.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" ht="166.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="5">
         <v>13</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6" t="s">
+      <c r="E17" s="5"/>
+      <c r="F17" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="G17" s="6"/>
-    </row>
-    <row r="18" spans="1:7" ht="193.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" ht="193.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="5">
         <v>14</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6" t="s">
+      <c r="E18" s="5"/>
+      <c r="F18" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="G18" s="6"/>
-    </row>
-    <row r="19" spans="1:7" ht="192.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" ht="192.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="5">
         <v>15</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6" t="s">
+      <c r="E19" s="5"/>
+      <c r="F19" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G19" s="6"/>
-    </row>
-    <row r="20" spans="1:7" ht="203.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" ht="203.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="5">
         <v>16</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6" t="s">
+      <c r="E20" s="5"/>
+      <c r="F20" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G20" s="6"/>
-    </row>
-    <row r="21" spans="1:7" ht="156.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" ht="156.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="5">
         <v>17</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6" t="s">
+      <c r="E21" s="5"/>
+      <c r="F21" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G21" s="6"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="5">
+        <v>18</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" s="11">
+        <v>19</v>
+      </c>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+    </row>
+    <row r="24" spans="1:8" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" s="14">
+        <v>20</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="52.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" s="14">
+        <v>21</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="H25" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.3">
+      <c r="A26" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B26" s="14">
+        <v>22</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.3">
+      <c r="A27" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" s="14">
+        <v>23</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.3">
+      <c r="A28" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28" s="14">
+        <v>24</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.3">
+      <c r="A29" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" s="14">
+        <v>25</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="G29" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="H29" s="14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.3">
+      <c r="A30" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="B30" s="14">
+        <v>27</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B31" s="5">
+        <v>28</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="H31" s="15" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="34.799999999999997" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B32" s="5">
+        <v>29</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="H32" s="15" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>

</xml_diff>